<commit_message>
Commit latest to github for moving to UFT 2021
</commit_message>
<xml_diff>
--- a/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
+++ b/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
@@ -20,10 +20,10 @@
     <t>BrowserName</t>
   </si>
   <si>
-    <t>CHROME</t>
-  </si>
-  <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>FIREFOX</t>
   </si>
   <si>
     <t>https://15.113.169.123:44300/sap/bc/ui5_ui5/ui2/ushell/shells/abap/FioriLaunchpad.html</t>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -549,7 +549,7 @@
         <v>7</v>
       </c>
       <c t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c t="s">
         <v>5</v>
@@ -557,7 +557,7 @@
     </row>
     <row>
       <c s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated datasheet to launch Chrome instead of Firefox
</commit_message>
<xml_diff>
--- a/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
+++ b/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
@@ -20,10 +20,10 @@
     <t>BrowserName</t>
   </si>
   <si>
+    <t>CHROME</t>
+  </si>
+  <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>FIREFOX</t>
   </si>
   <si>
     <t>https://15.113.169.123:44300/sap/bc/ui5_ui5/ui2/ushell/shells/abap/FioriLaunchpad.html</t>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -549,7 +549,7 @@
         <v>7</v>
       </c>
       <c t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s">
         <v>5</v>
@@ -557,7 +557,7 @@
     </row>
     <row>
       <c s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated to point where script runs without error
</commit_message>
<xml_diff>
--- a/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
+++ b/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>BrowserName</t>
   </si>
@@ -23,6 +23,9 @@
     <t>CHROME</t>
   </si>
   <si>
+    <t>dtCard</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
@@ -39,6 +42,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>Journal Entries to Be Verified</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -538,35 +544,42 @@
     <col min="2" max="2" width="74.2421875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.80859375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.40625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1">
-      <c t="s">
+    <row r="1" ht="14.95" customFormat="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s">
-        <v>2</v>
-      </c>
-      <c t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>3</v>
-      </c>
-      <c s="1" t="s">
-        <v>4</v>
-      </c>
-      <c s="3" t="s">
-        <v>6</v>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -587,7 +600,7 @@
     <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated data sheet to reflect new URL for the environment
</commit_message>
<xml_diff>
--- a/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
+++ b/uft-one-sap-fiori-general-ledger-overview/Default.xlsx
@@ -29,13 +29,13 @@
     <t>Username</t>
   </si>
   <si>
-    <t>https://15.113.169.123:44300/sap/bc/ui5_ui5/ui2/ushell/shells/abap/FioriLaunchpad.html</t>
-  </si>
-  <si>
     <t>S4H_FIN_DEM</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>https://sap-hana-vpn.mfdemoportal.com:44300/sap/bc/ui2/flp?sap-client=100&amp;sap-language=EN#Shell-home</t>
   </si>
   <si>
     <t>Welcome1</t>
@@ -532,13 +532,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.2421875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.04296875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.80859375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7890625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.40625" style="2" bestFit="1" customWidth="1"/>
@@ -556,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -567,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>

</xml_diff>